<commit_message>
Verbindung mit db geht und mann kann user erstellen
</commit_message>
<xml_diff>
--- a/MTCG/Checklist (5).xlsx
+++ b/MTCG/Checklist (5).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxpl\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxpl\Swen\SweShapeStack\MTCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429AEF32-959E-4772-B3AB-CB13D95A2B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2064938A-B94D-4786-BECC-FEC08BB66EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
@@ -239,7 +239,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,6 +249,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDADBDC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -265,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -275,6 +281,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -610,7 +617,7 @@
   <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -807,7 +814,7 @@
       <c r="A31" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="9">
         <v>3</v>
       </c>
     </row>
@@ -821,9 +828,7 @@
       <c r="A33" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="6">
-        <v>1</v>
-      </c>
+      <c r="C33" s="6"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
@@ -853,7 +858,7 @@
       <c r="A39" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="9">
         <v>2</v>
       </c>
     </row>
@@ -931,9 +936,7 @@
       <c r="A51" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C51" s="6">
-        <v>0.5</v>
-      </c>
+      <c r="C51" s="6"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
@@ -953,7 +956,7 @@
       </c>
       <c r="C54" s="2">
         <f>SUM(C21:C52)</f>
-        <v>48</v>
+        <v>46.5</v>
       </c>
     </row>
   </sheetData>
@@ -968,21 +971,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100495F7CC252815B47896F98900E10984C" ma:contentTypeVersion="2" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="afe1b3b164495dc81fdbcdcad6ec8b68">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="207955a2-a3fc-4582-b2ea-e4c7d1fb6048" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b6a42bf87c3f8727d31c248fc1697f6" ns2:_="">
     <xsd:import namespace="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
@@ -1114,10 +1102,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1139,19 +1152,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Packages können erstellt un aquired werden
</commit_message>
<xml_diff>
--- a/MTCG/Checklist (5).xlsx
+++ b/MTCG/Checklist (5).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxpl\Swen\SweShapeStack\MTCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2064938A-B94D-4786-BECC-FEC08BB66EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E260D115-DA5B-4AF3-A583-B79DFE617233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Checklist MonsterTradingCardsGame</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Describes design</t>
+  </si>
+  <si>
+    <t>check</t>
   </si>
 </sst>
 </file>
@@ -616,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -824,13 +827,13 @@
       </c>
       <c r="C32" s="6"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C33" s="6"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>29</v>
       </c>
@@ -838,7 +841,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
@@ -847,30 +850,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B38"/>
       <c r="C38"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C39" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>33</v>
       </c>
       <c r="C40" s="6">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>34</v>
       </c>
@@ -878,7 +887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>35</v>
       </c>
@@ -886,21 +895,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B44"/>
       <c r="C44" s="6"/>
     </row>
-    <row r="46" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>46</v>
       </c>
@@ -908,7 +917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>38</v>
       </c>
@@ -936,7 +945,9 @@
       <c r="A51" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C51" s="6"/>
+      <c r="C51" s="6">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
@@ -956,7 +967,7 @@
       </c>
       <c r="C54" s="2">
         <f>SUM(C21:C52)</f>
-        <v>46.5</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -971,6 +982,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100495F7CC252815B47896F98900E10984C" ma:contentTypeVersion="2" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="afe1b3b164495dc81fdbcdcad6ec8b68">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="207955a2-a3fc-4582-b2ea-e4c7d1fb6048" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b6a42bf87c3f8727d31c248fc1697f6" ns2:_="">
     <xsd:import namespace="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
@@ -1102,35 +1128,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1152,9 +1153,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Decks können konfiguriert und angezeigt werden
</commit_message>
<xml_diff>
--- a/MTCG/Checklist (5).xlsx
+++ b/MTCG/Checklist (5).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxpl\Swen\SweShapeStack\MTCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E260D115-DA5B-4AF3-A583-B79DFE617233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B04CFC6-9777-4276-BD37-BFEE8C87E822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>Checklist MonsterTradingCardsGame</t>
   </si>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -755,6 +755,9 @@
       <c r="C21" s="6">
         <v>3</v>
       </c>
+      <c r="D21" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
@@ -762,6 +765,9 @@
       </c>
       <c r="C22" s="6">
         <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -982,21 +988,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100495F7CC252815B47896F98900E10984C" ma:contentTypeVersion="2" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="afe1b3b164495dc81fdbcdcad6ec8b68">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="207955a2-a3fc-4582-b2ea-e4c7d1fb6048" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b6a42bf87c3f8727d31c248fc1697f6" ns2:_="">
     <xsd:import namespace="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
@@ -1128,10 +1119,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1153,19 +1169,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>